<commit_message>
reajuste na base de dados
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -163,6 +163,9 @@
     <t xml:space="preserve">Um dos jogos mais tristes que já joguei! É lindo! Vi capricho em cada pedacinho do jogo, muito boa a arte no geral!</t>
   </si>
   <si>
+    <t xml:space="preserve">Tristeza</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jogo muito mas muito mas muito lindo,uma verdadeira obra de arte...recomendo muito pra quem gosta de jogos que te envolvam emocionalmente!</t>
   </si>
   <si>
@@ -376,12 +379,12 @@
     <t xml:space="preserve">Você precisa de um controle, não gostei por causa disso</t>
   </si>
   <si>
+    <t xml:space="preserve">TRISTEZA</t>
+  </si>
+  <si>
     <t xml:space="preserve">EU ACHEI MUITO LINDA ESSA HISTÓRIA DEU ATÉ VONTADE DE CHORAR</t>
   </si>
   <si>
-    <t xml:space="preserve">TRISTEZA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eu fiquei triste pelo fato dos personagens terem uma historia de amor linda, e eu nunca tive nenhuma história</t>
   </si>
   <si>
@@ -545,9 +548,6 @@
   </si>
   <si>
     <t xml:space="preserve">Acho esse estilo de jogo super parado e lento, não tenho saco para ficar lendo essas histórinhas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tristeza</t>
   </si>
   <si>
     <t xml:space="preserve">Não é que o jogo é ruim, eu simplesmente não gostei...</t>
@@ -569,6 +569,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -650,11 +651,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A:B" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A:B"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1"/>
+  <tableColumns count="1">
     <tableColumn id="1" name="Comentarios"/>
-    <tableColumn id="2" name="Emoção"/>
   </tableColumns>
 </table>
 </file>
@@ -666,14 +666,14 @@
   </sheetPr>
   <dimension ref="A1:B174"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="199.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="93.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -1034,12 +1034,12 @@
         <v>46</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>3</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>3</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>3</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>3</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>3</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>3</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>3</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>3</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>3</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>3</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>3</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>3</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>3</v>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>3</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>3</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>3</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>3</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>3</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>3</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>3</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>3</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>3</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>3</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>3</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>3</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>3</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>3</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>3</v>
@@ -1279,335 +1279,335 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="B101" s="0" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>119</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B118" s="0" t="s">
         <v>119</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>119</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>119</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>119</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B122" s="0" t="s">
         <v>119</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B123" s="0" t="s">
         <v>119</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B124" s="0" t="s">
         <v>119</v>
@@ -1671,15 +1671,15 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B126" s="0" t="s">
         <v>119</v>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B127" s="0" t="s">
         <v>119</v>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>119</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>119</v>
@@ -1711,23 +1711,23 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B132" s="0" t="s">
         <v>119</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B133" s="0" t="s">
         <v>119</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B134" s="0" t="s">
         <v>119</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B135" s="0" t="s">
         <v>119</v>
@@ -1759,7 +1759,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B136" s="0" t="s">
         <v>119</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B137" s="0" t="s">
         <v>119</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B138" s="0" t="s">
         <v>119</v>
@@ -1783,15 +1783,15 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B140" s="0" t="s">
         <v>119</v>
@@ -1799,7 +1799,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B141" s="0" t="s">
         <v>119</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B142" s="0" t="s">
         <v>119</v>
@@ -1815,23 +1815,23 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B145" s="0" t="s">
         <v>119</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B146" s="0" t="s">
         <v>119</v>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B147" s="0" t="s">
         <v>119</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B148" s="0" t="s">
         <v>119</v>
@@ -1863,7 +1863,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B149" s="0" t="s">
         <v>119</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B150" s="0" t="s">
         <v>119</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B151" s="0" t="s">
         <v>119</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B152" s="0" t="s">
         <v>119</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B153" s="0" t="s">
         <v>119</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B154" s="0" t="s">
         <v>119</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B155" s="0" t="s">
         <v>119</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B156" s="0" t="s">
         <v>119</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B157" s="0" t="s">
         <v>119</v>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B158" s="0" t="s">
         <v>119</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B159" s="0" t="s">
         <v>119</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B160" s="0" t="s">
         <v>119</v>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B161" s="0" t="s">
         <v>119</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B162" s="0" t="s">
         <v>119</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B163" s="0" t="s">
         <v>119</v>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B164" s="0" t="s">
         <v>119</v>
@@ -1991,7 +1991,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B165" s="0" t="s">
         <v>119</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B166" s="0" t="s">
         <v>119</v>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B167" s="0" t="s">
         <v>119</v>
@@ -2015,7 +2015,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B168" s="0" t="s">
         <v>119</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B169" s="0" t="s">
         <v>119</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B170" s="0" t="s">
         <v>119</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B171" s="0" t="s">
         <v>119</v>
@@ -2047,10 +2047,10 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>175</v>
+        <v>47</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,7 +2058,7 @@
         <v>176</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>175</v>
+        <v>47</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,7 +2066,7 @@
         <v>177</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>175</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>